<commit_message>
fix layout issue fix height issue
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/chartFont.xlsx
+++ b/src/main/webapp/WEB-INF/books/chartFont.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BECF81-7CE4-E942-A838-31A4CB33F7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="18195" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20160" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChartFont" sheetId="1" r:id="rId1"/>
@@ -40,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -135,80 +141,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -220,16 +176,20 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US"/>
-              <a:t>分區各季營業額</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Volumn per Quater</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> per Region</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -244,6 +204,7 @@
       </c:layout>
       <c:areaChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -299,6 +260,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3277-C34C-89EF-3E442C618C1A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -355,6 +321,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3277-C34C-89EF-3E442C618C1A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -411,7 +382,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3277-C34C-89EF-3E442C618C1A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="75411840"/>
         <c:axId val="75413376"/>
       </c:areaChart>
@@ -420,22 +404,30 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="75413376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="75413376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="75411840"/>
         <c:crosses val="autoZero"/>
@@ -444,9 +436,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -473,7 +467,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -499,7 +499,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -534,7 +534,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,9 +566,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,6 +618,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -775,16 +811,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" thickBot="1">
+    <row r="1" spans="1:5" ht="19" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33.75" thickBot="1">
+    <row r="2" spans="1:5" ht="19" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -815,7 +851,7 @@
         <v>125678</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" thickBot="1">
+    <row r="3" spans="1:5" ht="19" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -832,7 +868,7 @@
         <v>157634</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="33.75" thickBot="1">
+    <row r="4" spans="1:5" ht="19" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>